<commit_message>
Add export scripts for all data types and update Excel files
- Add export-allocations.ts: exports allocations with employee and target names
- Add export-clients.ts: exports clients data
- Add export-projects.ts: exports projects data
- Add export-exceptions.ts: exports exceptions from API
- Add npm scripts for all export commands
- Update all data/*.xlsx files with current application data
- Add tmpclaude-* pattern to .gitignore

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/employees.xlsx
+++ b/data/employees.xlsx
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -831,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1222,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1256,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">

</xml_diff>

<commit_message>
Add vacation days import from יתרות חופשה.xlsx
Created import-vacation-days script to import vacation balances:

1. New Script: scripts/import-vacation-days.ts
   - Reads from data/יתרות חופשה.xlsx
   - Maps First Name + Last Name columns to employee names
   - Imports vacation balance from 'יתרה 31.12.2025' column
   - Case-insensitive employee name matching
   - Handles missing data gracefully

2. Import Results:
   - Updated 39 employees with vacation days
   - 8 billable employees now have >8 vacation days (VACATION exceptions)
   - Employees with high vacation: Verzhik Yana (14.95), Haimov Daniel (11.32),
     Peretz Yehonathan (10.25), Zuberi Moria (9.62), Yosefi Ori (9.34),
     Bendanan Nissim (9.16), Levin Yanir (8.5), Ratner Boris (8.05)

3. NPM Script:
   - Added "import-vacation-days" command to package.json

4. Updated employees.xlsx with imported vacation data

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/employees.xlsx
+++ b/data/employees.xlsx
@@ -437,7 +437,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -471,7 +471,7 @@
         <v>100</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>-5.25</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -522,7 +522,7 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -539,7 +539,7 @@
         <v>90</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>9.62</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -573,7 +573,7 @@
         <v>100</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>9.16</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>100</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -607,7 +607,7 @@
         <v>90</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3.58</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>100</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>100</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5.33</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>100</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -726,7 +726,7 @@
         <v>100</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -743,7 +743,7 @@
         <v>85</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>4.3</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -760,7 +760,7 @@
         <v>90</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>-5.54</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>100</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2.73</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -879,7 +879,7 @@
         <v>97</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>2.92</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -896,7 +896,7 @@
         <v>100</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>9.73</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>87</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1.94</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1049,7 +1049,7 @@
         <v>100</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>7.67</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>100</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>14.95</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1100,7 +1100,7 @@
         <v>100</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>-6.17</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1117,7 +1117,7 @@
         <v>100</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>11.32</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1134,7 +1134,7 @@
         <v>100</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>9.26</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1185,7 +1185,7 @@
         <v>80</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>9.34</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1202,7 +1202,7 @@
         <v>85</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>-5.02</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1253,7 +1253,7 @@
         <v>100</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>9.66</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1355,7 +1355,7 @@
         <v>100</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>-3.39</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1457,7 +1457,7 @@
         <v>100</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>10.25</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -1491,7 +1491,7 @@
         <v>100</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>1.67</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -1508,7 +1508,7 @@
         <v>100</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -1542,7 +1542,7 @@
         <v>100</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -1559,7 +1559,7 @@
         <v>100</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>-2.24</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>100</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>11.32</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -1610,7 +1610,7 @@
         <v>100</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1.83</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -1627,7 +1627,7 @@
         <v>100</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -1695,7 +1695,7 @@
         <v>100</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -1712,7 +1712,7 @@
         <v>100</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -1780,7 +1780,7 @@
         <v>100</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>8.05</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -1797,7 +1797,7 @@
         <v>100</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -1814,7 +1814,7 @@
         <v>100</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>3.26</v>
       </c>
       <c r="E83">
         <v>1</v>

</xml_diff>